<commit_message>
Update main.py and settings.py for BTC deposit and LBTC minting process
- Enhanced BTC deposit and LBTC minting workflow in main.py
- Added error handling and logging improvements
- Updated Soft_settings.xlsx with new BTC addresses
- Improved status management in settings.py
- Fixed bugs and optimized performance
</commit_message>
<xml_diff>
--- a/Soft_settings.xlsx
+++ b/Soft_settings.xlsx
@@ -2,56 +2,49 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozaytsev/Softs/CryptophileSoft/LombardSoft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5FD66F-4FCB-254A-86C9-DB1A718568A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53906B9-D1C9-5F4F-B75D-7BCE252C0DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="17180" xr2:uid="{D3C48D65-E016-784B-ABF3-8757E8BCDE93}"/>
+    <workbookView xWindow="4520" yWindow="620" windowWidth="18780" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Lombard" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>private_key</t>
   </si>
   <si>
+    <t>proxy</t>
+  </si>
+  <si>
     <t>max_gas_gwei</t>
   </si>
   <si>
     <t>exchange</t>
   </si>
   <si>
-    <t>OKX</t>
-  </si>
-  <si>
-    <t>Bitget</t>
+    <t>exchange_api_key</t>
+  </si>
+  <si>
+    <t>exchange_secret_key</t>
+  </si>
+  <si>
+    <t>exchange_passphrase</t>
+  </si>
+  <si>
+    <t>generate_btc_address</t>
   </si>
   <si>
     <t>btc_address</t>
@@ -73,28 +66,13 @@
   </si>
   <si>
     <t>Pendle</t>
-  </si>
-  <si>
-    <t>exchange_api_key</t>
-  </si>
-  <si>
-    <t>exchange_secret_key</t>
-  </si>
-  <si>
-    <t>exchange_passphrase</t>
-  </si>
-  <si>
-    <t>generate_btc_address</t>
-  </si>
-  <si>
-    <t>proxy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,16 +83,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,14 +102,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,107 +459,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F19DC3E-89F1-B841-B0D8-74080177BC81}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="V2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D1E360B0-BDA7-F54E-89B6-2EBBB9BA6C93}">
-      <formula1>$V$1:$V$2</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9690F385-D79C-AF46-9021-4D29543243FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F93E4D8D-64FE-8045-A817-6367894D7BD1}">
-      <formula1>0.0002</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>